<commit_message>
kosztorys - stan 29.05.2016
kosztorys - stan 29.05.2016
</commit_message>
<xml_diff>
--- a/Dokumentacja/kosztorys.xlsx
+++ b/Dokumentacja/kosztorys.xlsx
@@ -8,15 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
-    <sheet name="2" sheetId="2" r:id="rId2"/>
-    <sheet name="3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
   <si>
     <t>koszty zakupu oprogramowania</t>
   </si>
@@ -72,9 +70,6 @@
     <t>7.0.4</t>
   </si>
   <si>
-    <t>SAP Sybase PowerDesigner</t>
-  </si>
-  <si>
     <t>16.5</t>
   </si>
   <si>
@@ -169,9 +164,6 @@
   </si>
   <si>
     <t>łączny koszt utrzymania</t>
-  </si>
-  <si>
-    <t>IDE for Java EE Dev.</t>
   </si>
   <si>
     <t>pracownicy :
@@ -188,19 +180,22 @@
 10 000 zł / os.</t>
   </si>
   <si>
-    <t>czas realizacji projektu</t>
-  </si>
-  <si>
     <t>4 mies.</t>
   </si>
   <si>
     <t>łączny koszt realizacji projektu</t>
   </si>
   <si>
-    <t>365 Business Premium</t>
-  </si>
-  <si>
     <t>45 zł / mies.</t>
+  </si>
+  <si>
+    <t>Java EE Dev.</t>
+  </si>
+  <si>
+    <t>365 BP</t>
+  </si>
+  <si>
+    <t>SAP S. PowerDesigner</t>
   </si>
 </sst>
 </file>
@@ -403,7 +398,7 @@
     <xf numFmtId="6" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -415,6 +410,21 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -422,21 +432,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -733,7 +728,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:I11"/>
+  <dimension ref="B1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
@@ -742,27 +737,26 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="4.625" customWidth="1"/>
-    <col min="3" max="3" width="26.625" customWidth="1"/>
-    <col min="4" max="4" width="21.625" customWidth="1"/>
-    <col min="5" max="5" width="11.625" customWidth="1"/>
-    <col min="6" max="6" width="13.625" customWidth="1"/>
+    <col min="3" max="3" width="21.625" customWidth="1"/>
+    <col min="4" max="4" width="18.625" customWidth="1"/>
+    <col min="5" max="6" width="13.625" customWidth="1"/>
     <col min="7" max="7" width="6.625" customWidth="1"/>
-    <col min="8" max="8" width="21.625" customWidth="1"/>
+    <col min="8" max="8" width="13.625" customWidth="1"/>
     <col min="9" max="9" width="9.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15" thickBot="1"/>
+    <row r="1" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
     </row>
     <row r="3" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="B3" s="6" t="s">
@@ -784,7 +778,7 @@
         <v>8</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="I3" s="6" t="s">
         <v>9</v>
@@ -809,8 +803,8 @@
       <c r="G4" s="3">
         <v>5</v>
       </c>
-      <c r="H4" s="21" t="s">
-        <v>56</v>
+      <c r="H4" s="17" t="s">
+        <v>53</v>
       </c>
       <c r="I4" s="4">
         <f>PRODUCT(F4:G4)</f>
@@ -825,18 +819,18 @@
         <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G5" s="1">
         <v>5</v>
       </c>
-      <c r="H5" s="22"/>
+      <c r="H5" s="18"/>
       <c r="I5" s="2">
         <v>900</v>
       </c>
@@ -849,7 +843,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>14</v>
@@ -860,7 +854,7 @@
       <c r="G6" s="3">
         <v>4</v>
       </c>
-      <c r="H6" s="22"/>
+      <c r="H6" s="18"/>
       <c r="I6" s="4" t="s">
         <v>15</v>
       </c>
@@ -884,7 +878,7 @@
       <c r="G7" s="1">
         <v>5</v>
       </c>
-      <c r="H7" s="22"/>
+      <c r="H7" s="18"/>
       <c r="I7" s="2" t="s">
         <v>15</v>
       </c>
@@ -894,10 +888,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>10</v>
@@ -908,7 +902,7 @@
       <c r="G8" s="3">
         <v>1</v>
       </c>
-      <c r="H8" s="22"/>
+      <c r="H8" s="18"/>
       <c r="I8" s="4">
         <f>PRODUCT(F8:G8)</f>
         <v>10467</v>
@@ -919,21 +913,21 @@
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G9" s="1">
         <v>1</v>
       </c>
-      <c r="H9" s="22"/>
+      <c r="H9" s="18"/>
       <c r="I9" s="2">
         <v>760</v>
       </c>
@@ -943,7 +937,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>15</v>
@@ -952,19 +946,19 @@
         <v>10</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G10" s="3">
         <v>1</v>
       </c>
-      <c r="H10" s="23"/>
+      <c r="H10" s="19"/>
       <c r="I10" s="4">
         <v>76</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1">
       <c r="B11" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
@@ -977,364 +971,317 @@
         <v>15198</v>
       </c>
     </row>
+    <row r="12" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1"/>
+    <row r="13" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="B13" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="23"/>
+    </row>
+    <row r="14" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="B14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="B15" s="3">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="4">
+        <v>54</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="4">
+        <v>4914</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="B16" s="1">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="2">
+        <v>62</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="2">
+        <v>9300</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="B17" s="3">
+        <v>3</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="4">
+        <v>70</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="4">
+        <v>11550</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="B18" s="1">
+        <v>4</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="2">
+        <v>60</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="2">
+        <v>5100</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="B19" s="3">
+        <v>5</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="4">
+        <v>45</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="4">
+        <v>4050</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="B20" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="7">
+        <v>34914</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1"/>
+    <row r="22" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="B22" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+    </row>
+    <row r="23" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="B23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="B24" s="3">
+        <v>1</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="4">
+        <v>600</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="4">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="B25" s="1">
+        <v>2</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="2">
+        <v>400</v>
+      </c>
+      <c r="E25" s="18"/>
+      <c r="F25" s="2">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="B26" s="3">
+        <v>3</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="4">
+        <v>80</v>
+      </c>
+      <c r="E26" s="18"/>
+      <c r="F26" s="4">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="B27" s="1">
+        <v>4</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="2">
+        <v>300</v>
+      </c>
+      <c r="E27" s="18"/>
+      <c r="F27" s="2">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="B28" s="3">
+        <v>5</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="4">
+        <v>600</v>
+      </c>
+      <c r="E28" s="18"/>
+      <c r="F28" s="4">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="B29" s="1">
+        <v>6</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" s="2">
+        <v>81</v>
+      </c>
+      <c r="E29" s="18"/>
+      <c r="F29" s="2">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="B30" s="3">
+        <v>7</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30" s="18"/>
+      <c r="F30" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" ht="62.45" customHeight="1" thickBot="1">
+      <c r="B31" s="1">
+        <v>8</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E31" s="19"/>
+      <c r="F31" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="B32" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="7">
+        <v>176244</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1"/>
+    <row r="34" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
+      <c r="B34" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="11">
+        <v>226356</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="9">
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B32:E32"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="E24:E31"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B11:H11"/>
     <mergeCell ref="H4:H10"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B20:E20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:F9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col min="2" max="2" width="4.625" customWidth="1"/>
-    <col min="3" max="3" width="21.625" customWidth="1"/>
-    <col min="4" max="5" width="13.625" customWidth="1"/>
-    <col min="6" max="6" width="9.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:6" ht="15" thickBot="1"/>
-    <row r="2" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B2" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="18"/>
-    </row>
-    <row r="3" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="4">
-        <v>54</v>
-      </c>
-      <c r="F4" s="4">
-        <v>4914</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B5" s="1">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="2">
-        <v>62</v>
-      </c>
-      <c r="F5" s="2">
-        <v>9300</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B6" s="3">
-        <v>3</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="4">
-        <v>70</v>
-      </c>
-      <c r="F6" s="4">
-        <v>11550</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B7" s="1">
-        <v>4</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="2">
-        <v>60</v>
-      </c>
-      <c r="F7" s="2">
-        <v>5100</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B8" s="3">
-        <v>5</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="4">
-        <v>45</v>
-      </c>
-      <c r="F8" s="4">
-        <v>4050</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B9" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="7">
-        <v>34914</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B9:E9"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:F14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col min="2" max="2" width="4.625" customWidth="1"/>
-    <col min="3" max="3" width="21.625" customWidth="1"/>
-    <col min="4" max="4" width="18.625" customWidth="1"/>
-    <col min="5" max="5" width="21.625" customWidth="1"/>
-    <col min="6" max="6" width="10.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:6" ht="15" thickBot="1"/>
-    <row r="2" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B2" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-    </row>
-    <row r="3" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="4">
-        <v>600</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="4">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B5" s="1">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="2">
-        <v>400</v>
-      </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="2">
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B6" s="3">
-        <v>3</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="4">
-        <v>80</v>
-      </c>
-      <c r="E6" s="22"/>
-      <c r="F6" s="4">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B7" s="1">
-        <v>4</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="2">
-        <v>300</v>
-      </c>
-      <c r="E7" s="22"/>
-      <c r="F7" s="2">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B8" s="3">
-        <v>5</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="4">
-        <v>600</v>
-      </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="4">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B9" s="1">
-        <v>6</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="2">
-        <v>81</v>
-      </c>
-      <c r="E9" s="22"/>
-      <c r="F9" s="2">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B10" s="3">
-        <v>7</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="62.45" customHeight="1" thickBot="1">
-      <c r="B11" s="1">
-        <v>8</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B12" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="7">
-        <v>176244</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="15" thickBot="1"/>
-    <row r="14" spans="2:6" ht="20.100000000000001" customHeight="1" thickBot="1">
-      <c r="B14" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="11">
-        <v>226356</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="E4:E11"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="F11" numberStoredAsText="1"/>
+    <ignoredError sqref="F31" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>